<commit_message>
testdata and script change
</commit_message>
<xml_diff>
--- a/Data Files/tib.xlsx
+++ b/Data Files/tib.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D561DC61-47E1-4BC8-86F6-53E7674153C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6081114C-1DAD-40E4-A839-BBF8F2E3CD5E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>test</t>
   </si>
@@ -340,15 +340,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3"/>
+  <dimension ref="B3:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
script and eddata change
</commit_message>
<xml_diff>
--- a/Data Files/tib.xlsx
+++ b/Data Files/tib.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E16EB0-63BF-4110-9863-4CEB751C2BBA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1225BDA0-5CFA-412C-939B-CB356BD998C9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <t>test2</t>
   </si>
   <si>
-    <t>test1</t>
+    <t>test12</t>
   </si>
 </sst>
 </file>
@@ -349,7 +349,7 @@
   <dimension ref="B3:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>